<commit_message>
update run_id in WES xlsx templates
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FBC020-DACD-7142-948E-594EBADF157A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC74D752-CD02-5042-BB78-A0D63D66B317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="2900" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
     <t>germline.zip</t>
   </si>
   <si>
-    <t>run_1</t>
+    <t>test_prism_trial_id_run_1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
repair wes analysis corrupt file
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC74D752-CD02-5042-BB78-A0D63D66B317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A265FC6-BAB3-1040-B79F-E7F74EB9C190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="2900" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES Analysis" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -162,32 +162,32 @@
     <t>Germline</t>
   </si>
   <si>
+    <t>test_prism_trial_id_run_1</t>
+  </si>
+  <si>
     <t>test_prism_trial_id</t>
   </si>
   <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>tumor.zip</t>
-  </si>
-  <si>
-    <t>normal.zip</t>
-  </si>
-  <si>
-    <t>somatic.zip</t>
-  </si>
-  <si>
-    <t>germline.zip</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
+    <t>tumor</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>somatic</t>
+  </si>
+  <si>
+    <t>germline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,12 +206,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -294,10 +288,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -652,13 +646,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -668,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -682,20 +676,20 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -721,20 +715,20 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Revert "header width fix"
This reverts commit 19ef58eebefc38d72c230a13f7a1eb3d3d36c48a.
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5440E1A-8F65-064F-A052-01A445B0FF80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EF3C42-AA07-0648-8C20-F2DBA360AACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="11">
   <si>
     <t>#t</t>
   </si>
@@ -116,30 +116,12 @@
   <si>
     <t>test_prism_trial_id</t>
   </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>CTTTPP112.00</t>
-  </si>
-  <si>
-    <t>CTTTPP113.00</t>
-  </si>
-  <si>
-    <t>CTTTPP114.00</t>
-  </si>
-  <si>
-    <t>wes/analysis/1/</t>
-  </si>
-  <si>
-    <t>wes/analysis/2/</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,18 +141,6 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -238,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -246,11 +216,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +560,7 @@
   <dimension ref="A1:F205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -605,13 +573,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -628,11 +596,11 @@
       <c r="F2" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -652,28 +620,10 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
seperate neoantigen class 2 from run analysis
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64646AFE-2856-C94D-AE5E-66C3DBEAA32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2489F8E1-EFF6-0540-A31B-2F50D57C9B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -71,11 +71,24 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An id used for a paired analysis run.</t>
         </r>
       </text>
     </comment>
@@ -84,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="25">
   <si>
     <t>#t</t>
   </si>
@@ -116,6 +129,9 @@
     <t>Normal cimac id</t>
   </si>
   <si>
+    <t>Neoantigen mhc class ii analyzed</t>
+  </si>
+  <si>
     <t>LEGEND</t>
   </si>
   <si>
@@ -146,10 +162,10 @@
     <t>test_prism_trial_id</t>
   </si>
   <si>
+    <t>run_1</t>
+  </si>
+  <si>
     <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>run_1</t>
   </si>
   <si>
     <t>run_2</t>
@@ -162,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,12 +197,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -289,7 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -633,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,7 +655,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,8 +664,9 @@
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -663,18 +674,20 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -687,8 +700,11 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -696,67 +712,73 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1708,8 +1730,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1718,7 +1740,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E7"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1729,12 +1751,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -1742,15 +1764,15 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -1758,10 +1780,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -1769,13 +1791,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -1783,13 +1805,24 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
disallow process_as for FALSE values
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D48E68-6AF0-D543-9468-0AE644F1C6EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274B67C-2856-C14E-9767-C876DB10CB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,11 +311,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,7 +658,7 @@
   <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -671,12 +671,12 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -685,19 +685,19 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -730,7 +730,7 @@
         <v>23</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
make parse_through lambda functions
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274B67C-2856-C14E-9767-C876DB10CB16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EABF10F-9D08-3E42-9475-E73FB100D206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,7 +730,7 @@
         <v>23</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove neoantigen class 2
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588B3956-8855-014C-88C0-D95A6C886695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0C0B7E-87EA-764E-BC33-B244CAF9B7FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="5060" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES Analysis" sheetId="1" r:id="rId1"/>
@@ -79,25 +79,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Boolean to indicate whether Neoantigen MHC Class 2 analysis was performed: true/false</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="24">
   <si>
     <t>#t</t>
   </si>
@@ -129,9 +116,6 @@
     <t>Normal cimac id</t>
   </si>
   <si>
-    <t>Neoantigen mhc class ii</t>
-  </si>
-  <si>
     <t>LEGEND</t>
   </si>
   <si>
@@ -157,12 +141,6 @@
   </si>
   <si>
     <t>E.g. 'CTTTP01A1.00'</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Boolean to indicate whether Neoantigen MHC Class 2 analysis was performed: true/false</t>
   </si>
   <si>
     <t>run_1</t>
@@ -184,7 +162,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +185,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -221,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,12 +221,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5FA3F0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB2D2F6"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -311,12 +276,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E205"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -667,39 +630,36 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>26</v>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -712,85 +672,76 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1742,14 +1693,9 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E205" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"True,False"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -1757,7 +1703,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E8"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1768,12 +1714,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -1781,15 +1727,15 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -1797,10 +1743,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -1808,13 +1754,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -1822,24 +1768,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change example WES template to fix ordering in test
</commit_message>
<xml_diff>
--- a/template_examples/wes_analysis_template.xlsx
+++ b/template_examples/wes_analysis_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svn8\Documents\GitHub\cidc-schemas\template_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0C0B7E-87EA-764E-BC33-B244CAF9B7FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E0ADC7-7282-4A58-A0D6-BDB2CA11637E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="5060" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES Analysis" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -276,10 +276,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,26 +621,26 @@
   <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -652,14 +652,14 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -667,1026 +667,1026 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>6</v>
       </c>
@@ -1707,22 +1707,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1733,12 +1733,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1789,7 +1789,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>

</xml_diff>